<commit_message>
Bump version to v1.0.7 in mfgApp.js
</commit_message>
<xml_diff>
--- a/data/2026/ShiftCalendar_2026_Q1.xlsx
+++ b/data/2026/ShiftCalendar_2026_Q1.xlsx
@@ -923,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1069,47 +1069,41 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14343,8 +14337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D2A9D6-BB1E-4A7F-8469-30424B98EBCB}">
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="H20" zoomScaleNormal="40" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -14423,23 +14417,23 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
     <row r="4" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="6" t="s">
         <v>1</v>
       </c>
@@ -14460,18 +14454,18 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="13"/>
       <c r="W4" s="8"/>
     </row>
     <row r="5" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="14" t="s">
         <v>4</v>
       </c>
@@ -14507,18 +14501,18 @@
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="13"/>
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="51"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="21">
         <v>28</v>
       </c>
@@ -14559,7 +14553,7 @@
       <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="23" t="s">
@@ -14574,10 +14568,10 @@
       <c r="E7" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="57"/>
+      <c r="G7" s="58"/>
       <c r="H7" s="26" t="s">
         <v>60</v>
       </c>
@@ -14600,7 +14594,7 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A8" s="51"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
@@ -14641,7 +14635,7 @@
       <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A9" s="51"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="23" t="s">
         <v>16</v>
       </c>
@@ -14654,10 +14648,10 @@
       <c r="E9" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="58"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="29" t="s">
         <v>61</v>
       </c>
@@ -14680,7 +14674,7 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A10" s="51"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="23" t="s">
         <v>16</v>
       </c>
@@ -14721,7 +14715,7 @@
       <c r="W10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="55" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -14764,7 +14758,7 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A12" s="51"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="23" t="s">
         <v>16</v>
       </c>
@@ -14805,7 +14799,7 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="56" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="23" t="s">
@@ -14848,7 +14842,7 @@
       <c r="W13" s="3"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A14" s="52"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="23" t="s">
         <v>16</v>
       </c>
@@ -14975,7 +14969,7 @@
       <c r="W16" s="3"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="23" t="s">
@@ -15018,7 +15012,7 @@
       <c r="W17" s="3"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A18" s="51"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="23" t="s">
         <v>3</v>
       </c>
@@ -15109,15 +15103,15 @@
       <c r="W20" s="32"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="55" t="s">
+      <c r="A21" s="59"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
       <c r="H21" s="6" t="s">
         <v>1</v>
       </c>
@@ -15125,13 +15119,13 @@
         <f>I4+1</f>
         <v>2</v>
       </c>
-      <c r="J21" s="55" t="s">
+      <c r="J21" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
       <c r="O21" s="6" t="s">
         <v>1</v>
       </c>
@@ -15139,13 +15133,13 @@
         <f>I21+1</f>
         <v>3</v>
       </c>
-      <c r="Q21" s="55" t="s">
+      <c r="Q21" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
       <c r="V21" s="6" t="s">
         <v>1</v>
       </c>
@@ -15155,10 +15149,10 @@
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="53"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="14" t="s">
         <v>4</v>
       </c>
@@ -15224,10 +15218,10 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="51"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="21">
         <f>+I6+1</f>
         <v>4</v>
@@ -15314,48 +15308,48 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="59" t="s">
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="58" t="s">
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="59" t="s">
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="58" t="s">
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="59" t="s">
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
+      <c r="T24" s="54"/>
+      <c r="U24" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="V24" s="59"/>
-      <c r="W24" s="59"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A25" s="51"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="23" t="s">
         <v>3</v>
       </c>
@@ -15424,46 +15418,46 @@
       </c>
     </row>
     <row r="26" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A26" s="51"/>
+      <c r="A26" s="55"/>
       <c r="B26" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="60" t="s">
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="57" t="s">
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="60" t="s">
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="57" t="s">
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="60" t="s">
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="V26" s="60"/>
-      <c r="W26" s="60"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A27" s="51"/>
+      <c r="A27" s="55"/>
       <c r="B27" s="23" t="s">
         <v>16</v>
       </c>
@@ -15532,7 +15526,7 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="55" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="23" t="s">
@@ -15541,11 +15535,11 @@
       <c r="C28" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
       <c r="G28" s="24" t="s">
         <v>22</v>
       </c>
@@ -15555,26 +15549,26 @@
       <c r="I28" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
       <c r="M28" s="28" t="s">
         <v>25</v>
       </c>
       <c r="N28" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="O28" s="59" t="s">
+      <c r="O28" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="58" t="s">
+      <c r="P28" s="53"/>
+      <c r="Q28" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
       <c r="T28" s="28" t="s">
         <v>25</v>
       </c>
@@ -15589,43 +15583,43 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A29" s="51"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="D29" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="60" t="s">
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="57" t="s">
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
       <c r="M29" s="25" t="s">
         <v>23</v>
       </c>
       <c r="N29" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O29" s="60" t="s">
+      <c r="O29" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="57" t="s">
+      <c r="P29" s="57"/>
+      <c r="Q29" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="R29" s="57"/>
-      <c r="S29" s="57"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="58"/>
       <c r="T29" s="25" t="s">
         <v>23</v>
       </c>
@@ -15640,17 +15634,17 @@
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="56" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
       <c r="F30" s="28" t="s">
         <v>50</v>
       </c>
@@ -15663,26 +15657,26 @@
       <c r="I30" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="J30" s="58" t="s">
+      <c r="J30" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
       <c r="M30" s="28" t="s">
         <v>50</v>
       </c>
       <c r="N30" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="O30" s="59" t="s">
+      <c r="O30" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="58" t="s">
+      <c r="P30" s="53"/>
+      <c r="Q30" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="54"/>
       <c r="T30" s="28" t="s">
         <v>50</v>
       </c>
@@ -15697,43 +15691,43 @@
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A31" s="52"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
       <c r="F31" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="60" t="s">
+      <c r="G31" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="57" t="s">
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
       <c r="M31" s="25" t="s">
         <v>51</v>
       </c>
       <c r="N31" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="O31" s="60" t="s">
+      <c r="O31" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="57" t="s">
+      <c r="P31" s="57"/>
+      <c r="Q31" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="R31" s="57"/>
-      <c r="S31" s="57"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
       <c r="T31" s="25" t="s">
         <v>51</v>
       </c>
@@ -15754,39 +15748,39 @@
       <c r="B32" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C32" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
       <c r="F32" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="59" t="s">
+      <c r="G32" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="58" t="s">
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
       <c r="M32" s="28" t="s">
         <v>52</v>
       </c>
       <c r="N32" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O32" s="59" t="s">
+      <c r="O32" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="58" t="s">
+      <c r="P32" s="53"/>
+      <c r="Q32" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
       <c r="T32" s="28" t="s">
         <v>52</v>
       </c>
@@ -15810,36 +15804,36 @@
       <c r="C33" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="58" t="s">
+      <c r="D33" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="59" t="s">
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="58" t="s">
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
       <c r="M33" s="28" t="s">
         <v>39</v>
       </c>
       <c r="N33" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="O33" s="59" t="s">
+      <c r="O33" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="58" t="s">
+      <c r="P33" s="53"/>
+      <c r="Q33" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54"/>
       <c r="T33" s="28" t="s">
         <v>39</v>
       </c>
@@ -15854,7 +15848,7 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B34" s="23" t="s">
@@ -15925,7 +15919,7 @@
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A35" s="51"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="23" t="s">
         <v>3</v>
       </c>
@@ -16044,15 +16038,15 @@
       <c r="W37" s="32"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A38" s="53"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="55" t="s">
+      <c r="A38" s="59"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
       <c r="H38" s="6" t="s">
         <v>1</v>
       </c>
@@ -16090,10 +16084,10 @@
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="53"/>
+      <c r="B39" s="59"/>
       <c r="C39" s="14" t="s">
         <v>4</v>
       </c>
@@ -16159,10 +16153,10 @@
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="51"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="21">
         <f>+W23+1</f>
         <v>25</v>
@@ -16248,23 +16242,23 @@
       </c>
     </row>
     <row r="41" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="60" t="s">
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
       <c r="J41" s="36" t="s">
         <v>62</v>
       </c>
@@ -16277,11 +16271,11 @@
       <c r="M41" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="N41" s="60" t="s">
+      <c r="N41" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="O41" s="60"/>
-      <c r="P41" s="60"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="57"/>
       <c r="Q41" s="36" t="s">
         <v>62</v>
       </c>
@@ -16305,7 +16299,7 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A42" s="51"/>
+      <c r="A42" s="55"/>
       <c r="B42" s="23" t="s">
         <v>3</v>
       </c>
@@ -16374,21 +16368,21 @@
       </c>
     </row>
     <row r="43" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A43" s="51"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="59" t="s">
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
       <c r="J43" s="39" t="s">
         <v>66</v>
       </c>
@@ -16401,11 +16395,11 @@
       <c r="M43" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="N43" s="59" t="s">
+      <c r="N43" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="59"/>
-      <c r="P43" s="59"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
       <c r="Q43" s="39" t="s">
         <v>66</v>
       </c>
@@ -16429,7 +16423,7 @@
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A44" s="51"/>
+      <c r="A44" s="55"/>
       <c r="B44" s="23" t="s">
         <v>16</v>
       </c>
@@ -16498,7 +16492,7 @@
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="55" t="s">
         <v>21</v>
       </c>
       <c r="B45" s="23" t="s">
@@ -16507,11 +16501,11 @@
       <c r="C45" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="57" t="s">
+      <c r="D45" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
       <c r="G45" s="27" t="s">
         <v>24</v>
       </c>
@@ -16536,14 +16530,14 @@
       <c r="N45" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="O45" s="60" t="s">
+      <c r="O45" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="P45" s="60"/>
-      <c r="Q45" s="57" t="s">
+      <c r="P45" s="57"/>
+      <c r="Q45" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="R45" s="57"/>
+      <c r="R45" s="58"/>
       <c r="S45" s="25" t="s">
         <v>23</v>
       </c>
@@ -16561,18 +16555,18 @@
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A46" s="51"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C46" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="58" t="s">
+      <c r="D46" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
       <c r="G46" s="24" t="s">
         <v>22</v>
       </c>
@@ -16597,10 +16591,10 @@
       <c r="N46" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="O46" s="59" t="s">
+      <c r="O46" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="P46" s="59"/>
+      <c r="P46" s="53"/>
       <c r="Q46" s="28" t="s">
         <v>25</v>
       </c>
@@ -16624,7 +16618,7 @@
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="56" t="s">
         <v>26</v>
       </c>
       <c r="B47" s="23" t="s">
@@ -16633,10 +16627,10 @@
       <c r="C47" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="57" t="s">
+      <c r="D47" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E47" s="57"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="25" t="s">
         <v>51</v>
       </c>
@@ -16661,37 +16655,37 @@
       <c r="M47" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="N47" s="60" t="s">
+      <c r="N47" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="O47" s="60"/>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="57" t="s">
+      <c r="O47" s="57"/>
+      <c r="P47" s="57"/>
+      <c r="Q47" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="R47" s="57"/>
-      <c r="S47" s="57"/>
+      <c r="R47" s="58"/>
+      <c r="S47" s="58"/>
       <c r="T47" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="U47" s="60" t="s">
+      <c r="U47" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="V47" s="60"/>
-      <c r="W47" s="60"/>
+      <c r="V47" s="57"/>
+      <c r="W47" s="57"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A48" s="52"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="58" t="s">
+      <c r="D48" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="58"/>
+      <c r="E48" s="54"/>
       <c r="F48" s="28" t="s">
         <v>50</v>
       </c>
@@ -16716,24 +16710,24 @@
       <c r="M48" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N48" s="59" t="s">
+      <c r="N48" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="O48" s="59"/>
-      <c r="P48" s="59"/>
-      <c r="Q48" s="58" t="s">
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="R48" s="58"/>
-      <c r="S48" s="58"/>
+      <c r="R48" s="54"/>
+      <c r="S48" s="54"/>
       <c r="T48" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="U48" s="59" t="s">
+      <c r="U48" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="V48" s="59"/>
-      <c r="W48" s="59"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="53"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A49" s="20" t="s">
@@ -16745,10 +16739,10 @@
       <c r="C49" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="58" t="s">
+      <c r="D49" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="58"/>
+      <c r="E49" s="54"/>
       <c r="F49" s="28" t="s">
         <v>52</v>
       </c>
@@ -16773,24 +16767,24 @@
       <c r="M49" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="N49" s="59" t="s">
+      <c r="N49" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="O49" s="59"/>
-      <c r="P49" s="59"/>
-      <c r="Q49" s="58" t="s">
+      <c r="O49" s="53"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="R49" s="58"/>
-      <c r="S49" s="58"/>
+      <c r="R49" s="54"/>
+      <c r="S49" s="54"/>
       <c r="T49" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="U49" s="59" t="s">
+      <c r="U49" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="V49" s="59"/>
-      <c r="W49" s="59"/>
+      <c r="V49" s="53"/>
+      <c r="W49" s="53"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A50" s="20" t="s">
@@ -16802,11 +16796,11 @@
       <c r="C50" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D50" s="58" t="s">
+      <c r="D50" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
       <c r="G50" s="24" t="s">
         <v>38</v>
       </c>
@@ -16837,11 +16831,11 @@
       <c r="P50" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Q50" s="58" t="s">
+      <c r="Q50" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="R50" s="58"/>
-      <c r="S50" s="58"/>
+      <c r="R50" s="54"/>
+      <c r="S50" s="54"/>
       <c r="T50" s="42" t="s">
         <v>39</v>
       </c>
@@ -16856,7 +16850,7 @@
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B51" s="23" t="s">
@@ -16927,7 +16921,7 @@
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A52" s="51"/>
+      <c r="A52" s="55"/>
       <c r="B52" s="23" t="s">
         <v>3</v>
       </c>
@@ -17046,8 +17040,8 @@
       <c r="W54" s="32"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A55" s="53"/>
-      <c r="B55" s="54"/>
+      <c r="A55" s="59"/>
+      <c r="B55" s="61"/>
       <c r="C55" s="5" t="s">
         <v>53</v>
       </c>
@@ -17092,10 +17086,10 @@
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A56" s="53" t="s">
+      <c r="A56" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="53"/>
+      <c r="B56" s="59"/>
       <c r="C56" s="14" t="s">
         <v>4</v>
       </c>
@@ -17161,10 +17155,10 @@
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="51"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="21">
         <f>+W40+1</f>
         <v>15</v>
@@ -17250,18 +17244,18 @@
       </c>
     </row>
     <row r="58" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="58" t="s">
+      <c r="C58" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="54"/>
       <c r="G58" s="24" t="s">
         <v>57</v>
       </c>
@@ -17271,12 +17265,12 @@
       <c r="I58" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="J58" s="58" t="s">
+      <c r="J58" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="K58" s="58"/>
-      <c r="L58" s="58"/>
-      <c r="M58" s="58"/>
+      <c r="K58" s="54"/>
+      <c r="L58" s="54"/>
+      <c r="M58" s="54"/>
       <c r="N58" s="24" t="s">
         <v>57</v>
       </c>
@@ -17286,12 +17280,12 @@
       <c r="P58" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q58" s="58" t="s">
+      <c r="Q58" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="R58" s="58"/>
-      <c r="S58" s="58"/>
-      <c r="T58" s="58"/>
+      <c r="R58" s="54"/>
+      <c r="S58" s="54"/>
+      <c r="T58" s="54"/>
       <c r="U58" s="24" t="s">
         <v>57</v>
       </c>
@@ -17303,7 +17297,7 @@
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A59" s="51"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="23" t="s">
         <v>3</v>
       </c>
@@ -17372,16 +17366,16 @@
       </c>
     </row>
     <row r="60" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A60" s="51"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="57" t="s">
+      <c r="C60" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
       <c r="G60" s="27" t="s">
         <v>59</v>
       </c>
@@ -17391,12 +17385,12 @@
       <c r="I60" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="J60" s="61" t="s">
+      <c r="J60" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="K60" s="61"/>
-      <c r="L60" s="61"/>
-      <c r="M60" s="61"/>
+      <c r="K60" s="62"/>
+      <c r="L60" s="62"/>
+      <c r="M60" s="62"/>
       <c r="N60" s="27" t="s">
         <v>59</v>
       </c>
@@ -17406,12 +17400,12 @@
       <c r="P60" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="Q60" s="57" t="s">
+      <c r="Q60" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="R60" s="57"/>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
+      <c r="R60" s="58"/>
+      <c r="S60" s="58"/>
+      <c r="T60" s="58"/>
       <c r="U60" s="27" t="s">
         <v>59</v>
       </c>
@@ -17423,7 +17417,7 @@
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A61" s="51"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="23" t="s">
         <v>16</v>
       </c>
@@ -17492,7 +17486,7 @@
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="55" t="s">
         <v>21</v>
       </c>
       <c r="B62" s="23" t="s">
@@ -17563,7 +17557,7 @@
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A63" s="51"/>
+      <c r="A63" s="55"/>
       <c r="B63" s="23" t="s">
         <v>16</v>
       </c>
@@ -17632,7 +17626,7 @@
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A64" s="52" t="s">
+      <c r="A64" s="56" t="s">
         <v>26</v>
       </c>
       <c r="B64" s="23" t="s">
@@ -17641,10 +17635,10 @@
       <c r="C64" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="D64" s="58" t="s">
+      <c r="D64" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E64" s="58"/>
+      <c r="E64" s="54"/>
       <c r="F64" s="28" t="s">
         <v>50</v>
       </c>
@@ -17660,18 +17654,18 @@
       <c r="J64" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="K64" s="62" t="s">
+      <c r="K64" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="L64" s="62"/>
+      <c r="L64" s="60"/>
       <c r="M64" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="N64" s="59" t="s">
+      <c r="N64" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="O64" s="59"/>
-      <c r="P64" s="59"/>
+      <c r="O64" s="53"/>
+      <c r="P64" s="53"/>
       <c r="Q64" s="28" t="s">
         <v>32</v>
       </c>
@@ -17687,23 +17681,23 @@
       <c r="U64" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="V64" s="59" t="s">
+      <c r="V64" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="W64" s="59"/>
+      <c r="W64" s="53"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A65" s="52"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C65" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D65" s="57" t="s">
+      <c r="D65" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E65" s="57"/>
+      <c r="E65" s="58"/>
       <c r="F65" s="25" t="s">
         <v>51</v>
       </c>
@@ -17719,18 +17713,18 @@
       <c r="J65" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K65" s="61" t="s">
+      <c r="K65" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="L65" s="61"/>
+      <c r="L65" s="62"/>
       <c r="M65" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="N65" s="60" t="s">
+      <c r="N65" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="O65" s="60"/>
-      <c r="P65" s="60"/>
+      <c r="O65" s="57"/>
+      <c r="P65" s="57"/>
       <c r="Q65" s="25" t="s">
         <v>29</v>
       </c>
@@ -17763,10 +17757,10 @@
       <c r="C66" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D66" s="58" t="s">
+      <c r="D66" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E66" s="58"/>
+      <c r="E66" s="54"/>
       <c r="F66" s="28" t="s">
         <v>52</v>
       </c>
@@ -17782,18 +17776,18 @@
       <c r="J66" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="K66" s="62" t="s">
+      <c r="K66" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="L66" s="62"/>
+      <c r="L66" s="60"/>
       <c r="M66" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="N66" s="59" t="s">
+      <c r="N66" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="O66" s="59"/>
-      <c r="P66" s="59"/>
+      <c r="O66" s="53"/>
+      <c r="P66" s="53"/>
       <c r="Q66" s="28" t="s">
         <v>36</v>
       </c>
@@ -17806,10 +17800,10 @@
       <c r="T66" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="U66" s="59" t="s">
+      <c r="U66" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="V66" s="59"/>
+      <c r="V66" s="53"/>
       <c r="W66" s="24" t="s">
         <v>34</v>
       </c>
@@ -17886,7 +17880,7 @@
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A68" s="51" t="s">
+      <c r="A68" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B68" s="23" t="s">
@@ -17957,7 +17951,7 @@
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A69" s="51"/>
+      <c r="A69" s="55"/>
       <c r="B69" s="23" t="s">
         <v>3</v>
       </c>
@@ -18051,8 +18045,8 @@
       <c r="W70" s="3"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A71" s="53"/>
-      <c r="B71" s="54"/>
+      <c r="A71" s="59"/>
+      <c r="B71" s="61"/>
       <c r="C71" s="5" t="s">
         <v>54</v>
       </c>
@@ -18097,10 +18091,10 @@
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A72" s="53" t="s">
+      <c r="A72" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B72" s="53"/>
+      <c r="B72" s="59"/>
       <c r="C72" s="14" t="s">
         <v>4</v>
       </c>
@@ -18166,10 +18160,10 @@
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B73" s="51"/>
+      <c r="B73" s="55"/>
       <c r="C73" s="21">
         <f>W57+1</f>
         <v>8</v>
@@ -18256,18 +18250,18 @@
       </c>
     </row>
     <row r="74" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A74" s="51" t="s">
+      <c r="A74" s="55" t="s">
         <v>11</v>
       </c>
       <c r="B74" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="57" t="s">
+      <c r="C74" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D74" s="57"/>
-      <c r="E74" s="57"/>
-      <c r="F74" s="57"/>
+      <c r="D74" s="58"/>
+      <c r="E74" s="58"/>
+      <c r="F74" s="58"/>
       <c r="G74" s="27" t="s">
         <v>59</v>
       </c>
@@ -18277,31 +18271,31 @@
       <c r="I74" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J74" s="57" t="s">
+      <c r="J74" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="K74" s="57"/>
-      <c r="L74" s="57"/>
-      <c r="M74" s="57"/>
-      <c r="N74" s="60" t="s">
+      <c r="K74" s="58"/>
+      <c r="L74" s="58"/>
+      <c r="M74" s="58"/>
+      <c r="N74" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="O74" s="60"/>
-      <c r="P74" s="60"/>
-      <c r="Q74" s="57" t="s">
+      <c r="O74" s="57"/>
+      <c r="P74" s="57"/>
+      <c r="Q74" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="R74" s="57"/>
-      <c r="S74" s="57"/>
-      <c r="T74" s="57"/>
-      <c r="U74" s="60" t="s">
+      <c r="R74" s="58"/>
+      <c r="S74" s="58"/>
+      <c r="T74" s="58"/>
+      <c r="U74" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="V74" s="60"/>
-      <c r="W74" s="60"/>
+      <c r="V74" s="57"/>
+      <c r="W74" s="57"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A75" s="51"/>
+      <c r="A75" s="55"/>
       <c r="B75" s="23" t="s">
         <v>3</v>
       </c>
@@ -18370,16 +18364,16 @@
       </c>
     </row>
     <row r="76" spans="1:23" ht="36" x14ac:dyDescent="0.5">
-      <c r="A76" s="51"/>
+      <c r="A76" s="55"/>
       <c r="B76" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C76" s="58" t="s">
+      <c r="C76" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D76" s="58"/>
-      <c r="E76" s="58"/>
-      <c r="F76" s="58"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="54"/>
       <c r="G76" s="24" t="s">
         <v>57</v>
       </c>
@@ -18389,31 +18383,31 @@
       <c r="I76" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J76" s="58" t="s">
+      <c r="J76" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="K76" s="58"/>
-      <c r="L76" s="58"/>
-      <c r="M76" s="58"/>
-      <c r="N76" s="59" t="s">
+      <c r="K76" s="54"/>
+      <c r="L76" s="54"/>
+      <c r="M76" s="54"/>
+      <c r="N76" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="O76" s="59"/>
-      <c r="P76" s="59"/>
-      <c r="Q76" s="58" t="s">
+      <c r="O76" s="53"/>
+      <c r="P76" s="53"/>
+      <c r="Q76" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="R76" s="58"/>
-      <c r="S76" s="58"/>
-      <c r="T76" s="58"/>
-      <c r="U76" s="59" t="s">
+      <c r="R76" s="54"/>
+      <c r="S76" s="54"/>
+      <c r="T76" s="54"/>
+      <c r="U76" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="V76" s="59"/>
-      <c r="W76" s="59"/>
+      <c r="V76" s="53"/>
+      <c r="W76" s="53"/>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A77" s="51"/>
+      <c r="A77" s="55"/>
       <c r="B77" s="23" t="s">
         <v>16</v>
       </c>
@@ -18482,7 +18476,7 @@
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A78" s="51" t="s">
+      <c r="A78" s="55" t="s">
         <v>21</v>
       </c>
       <c r="B78" s="23" t="s">
@@ -18521,25 +18515,25 @@
       <c r="M78" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="N78" s="60" t="s">
+      <c r="N78" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="O78" s="60"/>
-      <c r="P78" s="60"/>
-      <c r="Q78" s="57" t="s">
+      <c r="O78" s="57"/>
+      <c r="P78" s="57"/>
+      <c r="Q78" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="R78" s="57"/>
-      <c r="S78" s="57"/>
-      <c r="T78" s="57"/>
-      <c r="U78" s="60" t="s">
+      <c r="R78" s="58"/>
+      <c r="S78" s="58"/>
+      <c r="T78" s="58"/>
+      <c r="U78" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="V78" s="60"/>
-      <c r="W78" s="60"/>
+      <c r="V78" s="57"/>
+      <c r="W78" s="57"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A79" s="51"/>
+      <c r="A79" s="55"/>
       <c r="B79" s="23" t="s">
         <v>16</v>
       </c>
@@ -18564,31 +18558,31 @@
       <c r="I79" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J79" s="58" t="s">
+      <c r="J79" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="K79" s="58"/>
-      <c r="L79" s="58"/>
-      <c r="M79" s="58"/>
-      <c r="N79" s="59" t="s">
+      <c r="K79" s="54"/>
+      <c r="L79" s="54"/>
+      <c r="M79" s="54"/>
+      <c r="N79" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="O79" s="59"/>
-      <c r="P79" s="59"/>
-      <c r="Q79" s="58" t="s">
+      <c r="O79" s="53"/>
+      <c r="P79" s="53"/>
+      <c r="Q79" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="R79" s="58"/>
-      <c r="S79" s="58"/>
-      <c r="T79" s="58"/>
-      <c r="U79" s="59" t="s">
+      <c r="R79" s="54"/>
+      <c r="S79" s="54"/>
+      <c r="T79" s="54"/>
+      <c r="U79" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="V79" s="59"/>
-      <c r="W79" s="59"/>
+      <c r="V79" s="53"/>
+      <c r="W79" s="53"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A80" s="52" t="s">
+      <c r="A80" s="56" t="s">
         <v>26</v>
       </c>
       <c r="B80" s="23" t="s">
@@ -18606,40 +18600,40 @@
       <c r="F80" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="G80" s="60" t="s">
+      <c r="G80" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H80" s="60"/>
-      <c r="I80" s="60"/>
-      <c r="J80" s="57" t="s">
+      <c r="H80" s="57"/>
+      <c r="I80" s="57"/>
+      <c r="J80" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="K80" s="57"/>
-      <c r="L80" s="57"/>
+      <c r="K80" s="58"/>
+      <c r="L80" s="58"/>
       <c r="M80" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="N80" s="60" t="s">
+      <c r="N80" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="O80" s="60"/>
-      <c r="P80" s="60"/>
-      <c r="Q80" s="57" t="s">
+      <c r="O80" s="57"/>
+      <c r="P80" s="57"/>
+      <c r="Q80" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="R80" s="57"/>
-      <c r="S80" s="57"/>
+      <c r="R80" s="58"/>
+      <c r="S80" s="58"/>
       <c r="T80" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="U80" s="60" t="s">
+      <c r="U80" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="V80" s="60"/>
-      <c r="W80" s="60"/>
+      <c r="V80" s="57"/>
+      <c r="W80" s="57"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A81" s="52"/>
+      <c r="A81" s="56"/>
       <c r="B81" s="23" t="s">
         <v>16</v>
       </c>
@@ -18655,37 +18649,37 @@
       <c r="F81" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="G81" s="59" t="s">
+      <c r="G81" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="H81" s="59"/>
-      <c r="I81" s="59"/>
-      <c r="J81" s="58" t="s">
+      <c r="H81" s="53"/>
+      <c r="I81" s="53"/>
+      <c r="J81" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="K81" s="58"/>
-      <c r="L81" s="58"/>
+      <c r="K81" s="54"/>
+      <c r="L81" s="54"/>
       <c r="M81" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="N81" s="59" t="s">
+      <c r="N81" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="O81" s="59"/>
-      <c r="P81" s="59"/>
-      <c r="Q81" s="58" t="s">
+      <c r="O81" s="53"/>
+      <c r="P81" s="53"/>
+      <c r="Q81" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="R81" s="58"/>
-      <c r="S81" s="58"/>
+      <c r="R81" s="54"/>
+      <c r="S81" s="54"/>
       <c r="T81" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="U81" s="59" t="s">
+      <c r="U81" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="V81" s="59"/>
-      <c r="W81" s="59"/>
+      <c r="V81" s="53"/>
+      <c r="W81" s="53"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A82" s="23" t="s">
@@ -18706,37 +18700,37 @@
       <c r="F82" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G82" s="59" t="s">
+      <c r="G82" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="H82" s="59"/>
-      <c r="I82" s="59"/>
-      <c r="J82" s="58" t="s">
+      <c r="H82" s="53"/>
+      <c r="I82" s="53"/>
+      <c r="J82" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="K82" s="58"/>
-      <c r="L82" s="58"/>
+      <c r="K82" s="54"/>
+      <c r="L82" s="54"/>
       <c r="M82" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="N82" s="59" t="s">
+      <c r="N82" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="O82" s="59"/>
-      <c r="P82" s="59"/>
-      <c r="Q82" s="58" t="s">
+      <c r="O82" s="53"/>
+      <c r="P82" s="53"/>
+      <c r="Q82" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="R82" s="58"/>
-      <c r="S82" s="58"/>
+      <c r="R82" s="54"/>
+      <c r="S82" s="54"/>
       <c r="T82" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="U82" s="59" t="s">
+      <c r="U82" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="V82" s="59"/>
-      <c r="W82" s="59"/>
+      <c r="V82" s="53"/>
+      <c r="W82" s="53"/>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.5">
       <c r="A83" s="20" t="s">
@@ -18778,25 +18772,25 @@
       <c r="M83" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="N83" s="59" t="s">
+      <c r="N83" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="O83" s="59"/>
-      <c r="P83" s="59"/>
-      <c r="Q83" s="58" t="s">
+      <c r="O83" s="53"/>
+      <c r="P83" s="53"/>
+      <c r="Q83" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="R83" s="58"/>
-      <c r="S83" s="58"/>
-      <c r="T83" s="58"/>
-      <c r="U83" s="59" t="s">
+      <c r="R83" s="54"/>
+      <c r="S83" s="54"/>
+      <c r="T83" s="54"/>
+      <c r="U83" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="V83" s="59"/>
-      <c r="W83" s="59"/>
+      <c r="V83" s="53"/>
+      <c r="W83" s="53"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A84" s="51" t="s">
+      <c r="A84" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B84" s="23" t="s">
@@ -18867,7 +18861,7 @@
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A85" s="51"/>
+      <c r="A85" s="55"/>
       <c r="B85" s="23" t="s">
         <v>3</v>
       </c>
@@ -18937,6 +18931,141 @@
     </row>
   </sheetData>
   <mergeCells count="159">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:T26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="N43:P43"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="U47:W47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="N48:P48"/>
+    <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="U48:W48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="U49:W49"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="C58:F58"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="Q58:T58"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="Q60:T60"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="Q50:S50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="N66:P66"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="N64:P64"/>
+    <mergeCell ref="V64:W64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="N76:P76"/>
+    <mergeCell ref="Q76:T76"/>
+    <mergeCell ref="U76:W76"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="N74:P74"/>
+    <mergeCell ref="N78:P78"/>
+    <mergeCell ref="Q78:T78"/>
+    <mergeCell ref="U78:W78"/>
+    <mergeCell ref="J79:M79"/>
+    <mergeCell ref="N79:P79"/>
+    <mergeCell ref="Q79:T79"/>
+    <mergeCell ref="U79:W79"/>
+    <mergeCell ref="Q74:T74"/>
+    <mergeCell ref="U74:W74"/>
     <mergeCell ref="J21:N21"/>
     <mergeCell ref="Q21:U21"/>
     <mergeCell ref="C38:G38"/>
@@ -18961,141 +19090,6 @@
     <mergeCell ref="N81:P81"/>
     <mergeCell ref="Q81:S81"/>
     <mergeCell ref="A78:A79"/>
-    <mergeCell ref="N78:P78"/>
-    <mergeCell ref="Q78:T78"/>
-    <mergeCell ref="U78:W78"/>
-    <mergeCell ref="J79:M79"/>
-    <mergeCell ref="N79:P79"/>
-    <mergeCell ref="Q79:T79"/>
-    <mergeCell ref="U79:W79"/>
-    <mergeCell ref="Q74:T74"/>
-    <mergeCell ref="U74:W74"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="N76:P76"/>
-    <mergeCell ref="Q76:T76"/>
-    <mergeCell ref="U76:W76"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="N74:P74"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="N66:P66"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="N64:P64"/>
-    <mergeCell ref="V64:W64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="Q58:T58"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="Q60:T60"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="Q50:S50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="U47:W47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="N48:P48"/>
-    <mergeCell ref="Q48:S48"/>
-    <mergeCell ref="U48:W48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="N49:P49"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="U49:W49"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="Q47:S47"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="N43:P43"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:S32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:T26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="C21:G21"/>
   </mergeCells>
   <conditionalFormatting sqref="A2 B3:W3 H4:S4 W4:W5 T4:U7 J5:N5 J6:S7 V6:W7 J9:K10 N9:U10 W9:W10 L9:M15 J17:W19 B19:I19 H20:L20 A21:A23 A24:C24 J24 N24 B25:F25 J25:P25 B26:C26 J26 N26 B27:F27 J27:P27 A70:W70">
     <cfRule type="cellIs" dxfId="1553" priority="3733" operator="equal">

</xml_diff>